<commit_message>
PR comments: fix test, improve test, rename var
</commit_message>
<xml_diff>
--- a/src/test/resources/network/brightspots/rcv/test_data/first_round_determines_threshold_test/first_round_determines_threshold_test_cvr.xlsx
+++ b/src/test/resources/network/brightspots/rcv/test_data/first_round_determines_threshold_test/first_round_determines_threshold_test_cvr.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="23">
   <si>
     <t xml:space="preserve">Cast Vote Record</t>
   </si>
@@ -85,10 +85,10 @@
     <t xml:space="preserve">Carmona, Ralph C. </t>
   </si>
   <si>
+    <t xml:space="preserve">Vail, Christopher L.</t>
+  </si>
+  <si>
     <t xml:space="preserve">Vail, Christopher L. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vail, Christopher L.</t>
   </si>
 </sst>
 </file>
@@ -194,17 +194,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:R19"/>
+  <dimension ref="A1:R1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2:E4"/>
+      <selection pane="topLeft" activeCell="D17" activeCellId="0" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.49"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="21.33"/>
   </cols>
   <sheetData>
@@ -266,7 +266,7 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B2" s="0" t="s">
         <v>18</v>
@@ -281,7 +281,7 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B3" s="0" t="s">
         <v>18</v>
@@ -292,10 +292,11 @@
       <c r="D3" s="0" t="s">
         <v>19</v>
       </c>
+      <c r="E3" s="2"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="n">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B4" s="0" t="s">
         <v>18</v>
@@ -307,9 +308,9 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="n">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B5" s="0" t="s">
         <v>18</v>
@@ -318,32 +319,26 @@
         <v>18</v>
       </c>
       <c r="D5" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="n">
+        <v>19</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="n">
         <v>20</v>
-      </c>
-      <c r="E5" s="0" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="n">
-        <v>20</v>
-      </c>
-      <c r="B6" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="C6" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="D6" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="E6" s="0" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="n">
-        <v>21</v>
       </c>
       <c r="B7" s="0" t="s">
         <v>18</v>
@@ -354,13 +349,10 @@
       <c r="D7" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="E7" s="0" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="n">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B8" s="0" t="s">
         <v>18</v>
@@ -375,9 +367,9 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="n">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B9" s="0" t="s">
         <v>18</v>
@@ -392,176 +384,145 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="E10" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="n">
         <v>24</v>
       </c>
-      <c r="B10" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="C10" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="D10" s="2" t="s">
+      <c r="B11" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="E11" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E12" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="n">
+        <v>26</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="D13" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="E10" s="0" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="n">
-        <v>25</v>
-      </c>
-      <c r="B11" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="C11" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="D11" s="0" t="s">
+      <c r="E13" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="n">
+        <v>27</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="D14" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="E14" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="C15" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="D15" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="E15" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="n">
+        <v>29</v>
+      </c>
+      <c r="B16" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="C16" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="D16" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="E16" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="B17" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="C17" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="D17" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="E11" s="0" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="n">
-        <v>26</v>
-      </c>
-      <c r="B12" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="C12" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="D12" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="E12" s="0" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="n">
-        <v>27</v>
-      </c>
-      <c r="B13" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="C13" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="D13" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="E13" s="0" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="n">
-        <v>28</v>
-      </c>
-      <c r="B14" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="C14" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="D14" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="E14" s="0" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="n">
-        <v>29</v>
-      </c>
-      <c r="B15" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="C15" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E15" s="0" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="n">
-        <v>30</v>
-      </c>
-      <c r="B16" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="C16" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="D16" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="E16" s="0" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="n">
-        <v>31</v>
-      </c>
-      <c r="B17" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="C17" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="D17" s="0" t="s">
-        <v>21</v>
-      </c>
       <c r="E17" s="0" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="n">
-        <v>32</v>
-      </c>
-      <c r="B18" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="C18" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="D18" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="E18" s="0" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="n">
-        <v>33</v>
-      </c>
-      <c r="B19" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="C19" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="D19" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="E19" s="0" t="s">
-        <v>19</v>
-      </c>
-    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>